<commit_message>
re-partition state county city
</commit_message>
<xml_diff>
--- a/Missing_counties_manual_checked_july 21 2023.xlsx
+++ b/Missing_counties_manual_checked_july 21 2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/state_county_city/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3988D946-9440-144F-9F2E-4947FDCF46DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C38801-D8AD-1242-A500-02D3788C7ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="500" windowWidth="41600" windowHeight="22380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7140" yWindow="500" windowWidth="37660" windowHeight="22380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Missing_counties123" sheetId="1" r:id="rId1"/>
@@ -5126,7 +5126,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
@@ -5167,13 +5167,10 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5535,8 +5532,8 @@
   <dimension ref="A1:K707"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I51" sqref="I51"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15763,7 +15760,7 @@
       <c r="F427">
         <v>38087</v>
       </c>
-      <c r="H427" s="20" t="s">
+      <c r="H427" s="4" t="s">
         <v>1406</v>
       </c>
       <c r="I427" s="4" t="s">
@@ -15789,7 +15786,7 @@
       <c r="F428">
         <v>38007</v>
       </c>
-      <c r="H428" s="20" t="s">
+      <c r="H428" s="4" t="s">
         <v>1314</v>
       </c>
     </row>
@@ -15812,7 +15809,7 @@
       <c r="F429">
         <v>38083</v>
       </c>
-      <c r="H429" s="20" t="s">
+      <c r="H429" s="4" t="s">
         <v>1408</v>
       </c>
     </row>
@@ -15835,7 +15832,7 @@
       <c r="F430">
         <v>38033</v>
       </c>
-      <c r="H430" s="20" t="s">
+      <c r="H430" s="4" t="s">
         <v>1314</v>
       </c>
     </row>

</xml_diff>